<commit_message>
slightly improve boa reanalyzed figure
</commit_message>
<xml_diff>
--- a/Part2 Reanalyzed Studies/Boa_ A Language and Infrastructure for Analyzing Ultra-Large-Scale Software Repositories/data.xlsx
+++ b/Part2 Reanalyzed Studies/Boa_ A Language and Infrastructure for Analyzing Ultra-Large-Scale Software Repositories/data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EFE794-9EE3-43E2-80C2-2FA10647A336}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 (Fig. 4 in Paper)" sheetId="1" r:id="rId1"/>
@@ -12,10 +13,18 @@
     <sheet name="Table 3 (Fig. 15 in paper)" sheetId="3" r:id="rId3"/>
     <sheet name="Tabelle1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -249,8 +258,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,8 +345,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -355,7 +364,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -812,7 +821,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -833,7 +842,7 @@
           <c:x val="0.14351609287198444"/>
           <c:y val="0.11338788935315106"/>
           <c:w val="0.78050623225813709"/>
-          <c:h val="0.74576110028688614"/>
+          <c:h val="0.70780718516132157"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1053,7 +1062,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1118,7 +1127,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1147,7 +1156,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35845694188434091"/>
+          <c:y val="0.91685436341853821"/>
+          <c:w val="0.27608459491650961"/>
+          <c:h val="7.5756077039940278E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1161,7 +1179,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1209,7 +1227,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2321,7 +2339,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2344,19 +2368,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>33130</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>16566</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>265341</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>153762</xdr:rowOff>
+      <xdr:colOff>612913</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2638,19 +2668,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2676,7 +2706,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -2704,7 +2734,7 @@
         <v>170.6829268292683</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2732,7 +2762,7 @@
         <v>90.232142857142861</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2760,7 +2790,7 @@
         <v>101.66666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2788,7 +2818,7 @@
         <v>78.576271186440678</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2816,7 +2846,7 @@
         <v>238.88888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2844,7 +2874,7 @@
         <v>216.42</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2872,7 +2902,7 @@
         <v>179.91379310344828</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2900,7 +2930,7 @@
         <v>168.24193548387098</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2928,7 +2958,7 @@
         <v>243.93023255813952</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2956,7 +2986,7 @@
         <v>239.04545454545453</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2984,7 +3014,7 @@
         <v>10.203389830508474</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3012,7 +3042,7 @@
         <v>11.823529411764707</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3040,7 +3070,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -3068,7 +3098,7 @@
         <v>12.086956521739131</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -3096,7 +3126,7 @@
         <v>10.772727272727273</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -3124,7 +3154,7 @@
         <v>9.1578947368421044</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3152,7 +3182,7 @@
         <v>8.2280701754385959</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -3180,7 +3210,7 @@
         <v>14.560975609756097</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3208,7 +3238,7 @@
         <v>10.595744680851064</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -3236,7 +3266,7 @@
         <v>8.71875</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -3264,12 +3294,12 @@
         <v>12.204081632653061</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -3298,7 +3328,7 @@
         <v>105.72058823529412</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3327,7 +3357,7 @@
         <v>210.07947019867549</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -3356,7 +3386,7 @@
         <v>11.001795332136446</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -3365,7 +3395,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -3394,7 +3424,7 @@
         <v>85.737535277516457</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -3406,7 +3436,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
     <sortCondition ref="A2:A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3415,16 +3445,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3444,7 +3474,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3465,7 +3495,7 @@
         <v>1116.9024390243903</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3486,7 +3516,7 @@
         <v>458.75</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -3507,7 +3537,7 @@
         <v>389.58333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -3528,7 +3558,7 @@
         <v>303.18644067796612</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3549,7 +3579,7 @@
         <v>2120.088888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3570,7 +3600,7 @@
         <v>1705.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -3591,7 +3621,7 @@
         <v>1650.9482758620691</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3612,7 +3642,7 @@
         <v>1426.4516129032259</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3633,7 +3663,7 @@
         <v>2346.1162790697676</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3654,12 +3684,12 @@
         <v>2006.340909090909</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3677,7 +3707,7 @@
         <v>529.75980392156862</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3695,13 +3725,13 @@
         <v>1834.523178807947</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3719,7 +3749,7 @@
         <v>1308.49209486166</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3732,14 +3762,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1"/>
+    <hyperlink ref="B19" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -3747,9 +3777,9 @@
       <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3773,7 +3803,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
@@ -3789,7 +3819,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>66</v>
       </c>
@@ -3805,7 +3835,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -3823,7 +3853,7 @@
         <v>6998</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
@@ -3839,7 +3869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>66</v>
       </c>
@@ -3855,7 +3885,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>66</v>
       </c>
@@ -3873,7 +3903,7 @@
         <v>5053</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
@@ -3889,7 +3919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
@@ -3905,7 +3935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>66</v>
       </c>
@@ -3929,7 +3959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>66</v>
       </c>
@@ -3961,7 +3991,7 @@
         <v>28.75</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
@@ -3995,7 +4025,7 @@
         <v>268.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>66</v>
       </c>
@@ -4029,7 +4059,7 @@
         <v>5391.75</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="7"/>
       <c r="C14" s="5"/>
@@ -4041,7 +4071,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -4072,7 +4102,7 @@
         <v>7.3636363636363633</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -4106,7 +4136,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -4139,11 +4169,11 @@
         <v>557.09090909090912</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4175,7 +4205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -4209,7 +4239,7 @@
         <v>560.83333333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -4243,7 +4273,7 @@
         <v>10574</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4259,7 +4289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -4275,7 +4305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -4293,7 +4323,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -4309,7 +4339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -4325,7 +4355,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -4343,7 +4373,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -4359,7 +4389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -4375,7 +4405,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -4393,7 +4423,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -4409,7 +4439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -4425,7 +4455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -4443,7 +4473,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -4459,7 +4489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -4475,7 +4505,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -4493,7 +4523,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -4509,7 +4539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -4525,7 +4555,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -4543,7 +4573,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -4559,7 +4589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -4575,7 +4605,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -4593,7 +4623,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -4609,7 +4639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -4625,7 +4655,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>27</v>
       </c>
@@ -4643,7 +4673,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -4659,7 +4689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -4675,7 +4705,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -4693,7 +4723,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>67</v>
       </c>
@@ -4709,7 +4739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>67</v>
       </c>
@@ -4725,7 +4755,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>67</v>
       </c>
@@ -4743,7 +4773,7 @@
         <v>10750</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>67</v>
       </c>
@@ -4759,7 +4789,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>67</v>
       </c>
@@ -4775,7 +4805,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>67</v>
       </c>
@@ -4793,7 +4823,7 @@
         <v>10821</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>67</v>
       </c>
@@ -4809,7 +4839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>67</v>
       </c>
@@ -4825,7 +4855,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>67</v>
       </c>
@@ -4843,7 +4873,7 @@
         <v>10435</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>67</v>
       </c>
@@ -4859,7 +4889,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>67</v>
       </c>
@@ -4875,7 +4905,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>67</v>
       </c>
@@ -4893,7 +4923,7 @@
         <v>10431</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>67</v>
       </c>
@@ -4909,7 +4939,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>67</v>
       </c>
@@ -4925,7 +4955,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>67</v>
       </c>
@@ -4943,7 +4973,7 @@
         <v>10489</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>67</v>
       </c>
@@ -4959,7 +4989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>67</v>
       </c>
@@ -4975,7 +5005,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>67</v>
       </c>
@@ -4993,68 +5023,68 @@
         <v>10518</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="2:2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="2:2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="2:2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A1:E84">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E84">
     <sortCondition ref="A1:A84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5063,14 +5093,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>